<commit_message>
Updated metascape results for updated CD62L- resident Treg analysis.
Replaced mousepool correction by prep-batch correction for colon vs. non-colon DGE analysis in CD62L- resident Treg. Added 2 more barcode plots for the top 4 enriched hallmark gene sets in total. Switched to granular design with pre-batch correction as in updated batch-corrected data for barplots. Updated barplots for enriched barplots along with updated metascape results. Updated scatterplots for single calls to geom_point and geom_text_repel.

Implemented granular design in cvnc pc analysis, however more stringent filtering based on colon vs. non-colon (equivalent to organ identity in that case). Updated scatterplots and barcode plots for best plotting at the moment.

Implemented granular design in pvc organ-wise comparisons, adjusting for poly or allo affiliation. Respective Scatterplots and barcode plots are updated as well in terms of correctly rounded p-values as well as more soft-coded plotting for DEGs.
</commit_message>
<xml_diff>
--- a/bulkRNAseq_analyses/METASCAPE/SupplementaryFigure3g_cluster3.spleen.up_metascape_result.xlsx
+++ b/bulkRNAseq_analyses/METASCAPE/SupplementaryFigure3g_cluster3.spleen.up_metascape_result.xlsx
@@ -534,7 +534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>GeneSymbol</t>
+          <t>MyList</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -580,34 +580,39 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>ko04970 Salivary secretion</t>
+          <t>GO:0051588 regulation of neurotransmitter</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>GO:0006936 muscle contraction</t>
+          <t>mmu04970 Salivary secretion</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>GO:0051588 regulation of neurotransmitter</t>
+          <t>GO:0060326 cell chemotaxis</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>GO:1903530 regulation of secretion by cel</t>
+          <t>GO:0072593 reactive oxygen species metabo</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>GO:0031175 neuron projection development</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dlg3</t>
+          <t>Cd200</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>53310</t>
+          <t>17470</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -622,7 +627,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>53310</t>
+          <t>17470</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -637,7 +642,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -651,6 +656,11 @@
         </is>
       </c>
       <c r="K2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -659,12 +669,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rec8</t>
+          <t>Egr2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>56739</t>
+          <t>13654</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -679,7 +689,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>56739</t>
+          <t>13654</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -699,29 +709,34 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>0.0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tmem38b</t>
+          <t>Npas4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>52076</t>
+          <t>225872</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -736,7 +751,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>52076</t>
+          <t>225872</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -756,7 +771,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -765,6 +780,11 @@
         </is>
       </c>
       <c r="K4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -773,12 +793,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Slc12a2</t>
+          <t>Actg2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>20496</t>
+          <t>11468</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -793,7 +813,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20496</t>
+          <t>11468</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -803,19 +823,19 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>0.0</t>
@@ -823,19 +843,24 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Slc7a10</t>
+          <t>Egr3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>53896</t>
+          <t>13655</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -850,7 +875,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>53896</t>
+          <t>13655</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -875,10 +900,15 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -887,12 +917,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tiam1</t>
+          <t>Ighd</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21844</t>
+          <t>380797</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -907,7 +937,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>21844</t>
+          <t>380797</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -936,6 +966,11 @@
         </is>
       </c>
       <c r="K7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -944,12 +979,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Rragd</t>
+          <t>Scarna13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>52187</t>
+          <t>100306943</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -964,7 +999,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>52187</t>
+          <t>100306943</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -993,6 +1028,11 @@
         </is>
       </c>
       <c r="K8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1001,12 +1041,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Atp9a</t>
+          <t>Gm22442</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11981</t>
+          <t>115487906</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1021,7 +1061,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>11981</t>
+          <t>115487906</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1046,24 +1086,29 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Prag1</t>
+          <t>Gpm6b</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>244418</t>
+          <t>14758</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1078,7 +1123,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>244418</t>
+          <t>14758</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1093,7 +1138,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1109,23 +1154,28 @@
       <c r="K10" t="inlineStr">
         <is>
           <t>0.0</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Fam160a1</t>
+          <t>Ddx43</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>229488</t>
+          <t>100048658</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>gene_synonym</t>
+          <t>symbol</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1135,7 +1185,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>229488</t>
+          <t>100048658</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1164,6 +1214,11 @@
         </is>
       </c>
       <c r="K11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1172,12 +1227,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ttn</t>
+          <t>Dlg3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>22138</t>
+          <t>53310</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1192,7 +1247,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>22138</t>
+          <t>53310</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1202,7 +1257,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1212,7 +1267,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1222,19 +1277,24 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Usp11</t>
+          <t>Rec8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>236733</t>
+          <t>56739</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1249,7 +1309,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>236733</t>
+          <t>56739</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1278,6 +1338,11 @@
         </is>
       </c>
       <c r="K13" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1286,12 +1351,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Arhgap39</t>
+          <t>Prkca</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>223666</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1306,7 +1371,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>223666</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1321,34 +1386,39 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>0.0</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tbc1d4</t>
+          <t>Zfp827</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>210789</t>
+          <t>622675</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1363,7 +1433,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>210789</t>
+          <t>622675</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1388,10 +1458,15 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1400,12 +1475,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nrn1</t>
+          <t>Pacsin1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>68404</t>
+          <t>23969</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1420,7 +1495,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>68404</t>
+          <t>23969</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1435,7 +1510,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1445,10 +1520,15 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
@@ -1457,12 +1537,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hivep3</t>
+          <t>Cybb</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16656</t>
+          <t>13058</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1477,7 +1557,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>16656</t>
+          <t>13058</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1506,6 +1586,11 @@
         </is>
       </c>
       <c r="K17" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1514,12 +1599,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cst7</t>
+          <t>Nrn1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>13011</t>
+          <t>68404</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1534,7 +1619,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13011</t>
+          <t>68404</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1544,39 +1629,44 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="I18" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>1.0</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Gdpd5</t>
+          <t>Tspan3</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>233552</t>
+          <t>56434</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1591,7 +1681,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>233552</t>
+          <t>56434</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1620,6 +1710,11 @@
         </is>
       </c>
       <c r="K19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1628,12 +1723,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Naip6</t>
+          <t>Bmyc</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17952</t>
+          <t>107771</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1648,7 +1743,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>17952</t>
+          <t>107771</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1658,7 +1753,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1677,6 +1772,11 @@
         </is>
       </c>
       <c r="K20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1685,12 +1785,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Naip5</t>
+          <t>Ephx1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17951</t>
+          <t>13849</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1705,7 +1805,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>17951</t>
+          <t>13849</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1715,7 +1815,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1734,6 +1834,11 @@
         </is>
       </c>
       <c r="K21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1742,12 +1847,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gm3739</t>
+          <t>Ppat</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>100042235</t>
+          <t>231327</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1762,7 +1867,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>100042235</t>
+          <t>231327</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1791,6 +1896,11 @@
         </is>
       </c>
       <c r="K22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1799,12 +1909,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Clip2</t>
+          <t>Cbx6</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>269713</t>
+          <t>494448</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1819,7 +1929,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>269713</t>
+          <t>494448</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1848,6 +1958,11 @@
         </is>
       </c>
       <c r="K23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1856,12 +1971,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Tnfrsf8</t>
+          <t>Izumo1r</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21941</t>
+          <t>64931</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1876,7 +1991,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>21941</t>
+          <t>64931</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1905,6 +2020,11 @@
         </is>
       </c>
       <c r="K24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1913,12 +2033,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Npas4</t>
+          <t>Cul7</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>225872</t>
+          <t>66515</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1933,7 +2053,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>225872</t>
+          <t>66515</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1962,6 +2082,11 @@
         </is>
       </c>
       <c r="K25" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1970,17 +2095,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Gucy1a3</t>
+          <t>Cxcr5</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>60596</t>
+          <t>12145</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>gene_synonym</t>
+          <t>symbol</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1990,7 +2115,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>60596</t>
+          <t>12145</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2005,20 +2130,25 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="K26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2027,12 +2157,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ighd</t>
+          <t>Usp11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>380797</t>
+          <t>236733</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2047,7 +2177,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>380797</t>
+          <t>236733</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2076,6 +2206,11 @@
         </is>
       </c>
       <c r="K27" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2084,12 +2219,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Gpm6b</t>
+          <t>Arhgap39</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>14758</t>
+          <t>223666</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2104,7 +2239,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>14758</t>
+          <t>223666</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2119,7 +2254,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2129,10 +2264,15 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2141,12 +2281,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Ddx43</t>
+          <t>Gm26202</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>100048658</t>
+          <t>115488998</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2161,7 +2301,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>100048658</t>
+          <t>115488998</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2190,6 +2330,11 @@
         </is>
       </c>
       <c r="K29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2198,49 +2343,74 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Gm17173</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
+          <t>Snord82</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>80828</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>80828</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>H2-Oa</t>
+          <t>Snord87</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>15001</t>
+          <t>266793</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2255,7 +2425,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>15001</t>
+          <t>266793</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2284,6 +2454,11 @@
         </is>
       </c>
       <c r="K31" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2292,12 +2467,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tspan3</t>
+          <t>Snord32a</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>56434</t>
+          <t>27209</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2312,7 +2487,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>56434</t>
+          <t>27209</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2341,6 +2516,11 @@
         </is>
       </c>
       <c r="K32" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2349,12 +2529,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bmyc</t>
+          <t>Snord34</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>107771</t>
+          <t>27210</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2369,7 +2549,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>107771</t>
+          <t>27210</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2398,6 +2578,11 @@
         </is>
       </c>
       <c r="K33" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2406,12 +2591,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Ephx1</t>
+          <t>Tbc1d4</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13849</t>
+          <t>210789</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2426,7 +2611,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>13849</t>
+          <t>210789</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2441,7 +2626,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2455,6 +2640,11 @@
         </is>
       </c>
       <c r="K34" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2463,12 +2653,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ppat</t>
+          <t>Gm3739</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>231327</t>
+          <t>100042235</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2483,7 +2673,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>231327</t>
+          <t>100042235</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2512,6 +2702,11 @@
         </is>
       </c>
       <c r="K35" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2520,12 +2715,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Cbx6</t>
+          <t>Hivep3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>494448</t>
+          <t>16656</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2540,7 +2735,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>494448</t>
+          <t>16656</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2569,6 +2764,11 @@
         </is>
       </c>
       <c r="K36" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2577,12 +2777,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Izumo1r</t>
+          <t>Cst7</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>64931</t>
+          <t>13011</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2597,7 +2797,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>64931</t>
+          <t>13011</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2607,7 +2807,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2617,7 +2817,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2626,6 +2826,11 @@
         </is>
       </c>
       <c r="K37" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2634,12 +2839,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Cybb</t>
+          <t>Chn2</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>13058</t>
+          <t>69993</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2654,7 +2859,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>13058</t>
+          <t>69993</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2669,7 +2874,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2683,6 +2888,11 @@
         </is>
       </c>
       <c r="K38" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2691,12 +2901,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Cxcr5</t>
+          <t>Slc12a2</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>12145</t>
+          <t>20496</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2711,7 +2921,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>12145</t>
+          <t>20496</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2721,7 +2931,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2731,15 +2941,20 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2748,12 +2963,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Prkca</t>
+          <t>Slc7a10</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>18750</t>
+          <t>53896</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2768,7 +2983,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>18750</t>
+          <t>53896</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2783,34 +2998,39 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Zfp827</t>
+          <t>Naip6</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>622675</t>
+          <t>17952</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2825,7 +3045,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>622675</t>
+          <t>17952</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2835,7 +3055,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2854,6 +3074,11 @@
         </is>
       </c>
       <c r="K41" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2862,12 +3087,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Pacsin1</t>
+          <t>Naip5</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>23969</t>
+          <t>17951</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2882,7 +3107,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>23969</t>
+          <t>17951</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2892,7 +3117,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2907,22 +3132,917 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Gdpd5</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>233552</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>233552</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Atp9a</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>11981</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>11981</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Rgs16</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>19734</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>19734</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Mctp1</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>78771</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>78771</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Myo1h</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>231646</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>231646</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Chst15</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>77590</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>77590</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Gucy1a3</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>60596</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>gene_synonym</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>60596</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Prag1</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>244418</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>244418</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Rragd</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>52187</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>52187</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Gm37347</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>AC154627.3</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Tnfrsf8</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>21941</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>21941</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Susd2</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>71733</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>71733</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Fam160a1</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>229488</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>gene_synonym</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>229488</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ttn</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>22138</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>22138</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E42">
+  <conditionalFormatting sqref="E2:E57">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G57">
     <cfRule type="cellIs" priority="2" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2933,7 +4053,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H42">
+  <conditionalFormatting sqref="H2:H57">
     <cfRule type="cellIs" priority="5" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2944,7 +4064,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I42">
+  <conditionalFormatting sqref="I2:I57">
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2955,7 +4075,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J42">
+  <conditionalFormatting sqref="J2:J57">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2966,7 +4086,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K42">
+  <conditionalFormatting sqref="K2:K57">
     <cfRule type="cellIs" priority="14" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2974,6 +4094,17 @@
       <formula>"1"</formula>
     </cfRule>
     <cfRule type="expression" priority="16" dxfId="2" stopIfTrue="1">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L57">
+    <cfRule type="cellIs" priority="17" operator="equal" dxfId="1" stopIfTrue="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="18" operator="equal" dxfId="1" stopIfTrue="0">
+      <formula>"1"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="19" dxfId="2" stopIfTrue="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2989,7 +4120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3066,14 +4197,14 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-4.1199323855</v>
+        <v>-3.8865642647</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4/49</t>
+          <t>4/44</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -3109,14 +4240,14 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-4.1199323855</v>
+        <v>-3.8865642647</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4/49</t>
+          <t>4/44</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -3152,7 +4283,7 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-2.542707383</v>
+        <v>-2.2431293242</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
@@ -3195,7 +4326,7 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>-2.3219637852</v>
+        <v>-2.0273283633</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -3219,7 +4350,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1_Member</t>
+          <t>2_Summary</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3229,76 +4360,76 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>GO:0010466</t>
+          <t>GO:0051588</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>negative regulation of peptidase activity</t>
+          <t>regulation of neurotransmitter transport</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>-2.1521158653</v>
+        <v>-3.8480472385</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3/84</t>
+          <t>4/45</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>13011,17951,17952</t>
+          <t>14758,18750,68404,78771,11981,17470,23969,210789,20496,22138,225872</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Cst7,Naip5,Naip6</t>
+          <t>Gpm6b,Prkca,Nrn1,Mctp1,Atp9a,Cd200,Pacsin1,Tbc1d4,Slc12a2,Ttn,Npas4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2_Summary</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>KEGG Pathway</t>
+          <t>GO Biological Processes</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ko04970</t>
+          <t>GO:0051588</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Salivary secretion</t>
+          <t>regulation of neurotransmitter transport</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>-3.3626075359</v>
+        <v>-3.8480472385</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3/32</t>
+          <t>4/45</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>18750,20496,60596,13058,14758,52076,12145</t>
+          <t>14758,18750,68404,78771</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Prkca,Slc12a2,Gucy1a1,Cybb,Gpm6b,Tmem38b,Cxcr5</t>
+          <t>Gpm6b,Prkca,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
@@ -3310,38 +4441,38 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KEGG Pathway</t>
+          <t>GO Biological Processes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ko04970</t>
+          <t>GO:0051051</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Salivary secretion</t>
+          <t>negative regulation of transport</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-3.3626075359</v>
+        <v>-3.3411377526</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3/32</t>
+          <t>7/235</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>18750,20496,60596</t>
+          <t>11981,14758,17470,18750,23969,78771,210789</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Prkca,Slc12a2,Gucy1a1</t>
+          <t>Atp9a,Gpm6b,Cd200,Prkca,Pacsin1,Mctp1,Tbc1d4</t>
         </is>
       </c>
     </row>
@@ -3353,38 +4484,38 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>KEGG Pathway</t>
+          <t>GO Biological Processes</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mmu04970</t>
+          <t>GO:0001505</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Salivary secretion</t>
+          <t>regulation of neurotransmitter levels</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>-3.322624285</v>
+        <v>-3.0833540895</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3/33</t>
+          <t>4/71</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>18750,20496,60596</t>
+          <t>14758,18750,68404,78771</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Prkca,Slc12a2,Gucy1a1</t>
+          <t>Gpm6b,Prkca,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
@@ -3401,33 +4532,33 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GO:0043269</t>
+          <t>GO:1903530</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>regulation of ion transport</t>
+          <t>regulation of secretion by cell</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>-2.270018949</v>
+        <v>-3.0596733891</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>5/244</t>
+          <t>7/262</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>13058,14758,18750,20496,52076</t>
+          <t>11981,17470,18750,20496,22138,68404,78771</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Cybb,Gpm6b,Prkca,Slc12a2,Tmem38b</t>
+          <t>Atp9a,Cd200,Prkca,Slc12a2,Ttn,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
@@ -3444,40 +4575,40 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GO:0030595</t>
+          <t>GO:0051046</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>leukocyte chemotaxis</t>
+          <t>regulation of secretion</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>-2.0178765907</v>
+        <v>-2.8999295696</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3/94</t>
+          <t>7/279</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>12145,18750,20496</t>
+          <t>11981,17470,18750,20496,22138,68404,78771</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Cxcr5,Prkca,Slc12a2</t>
+          <t>Atp9a,Cd200,Prkca,Slc12a2,Ttn,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3_Summary</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3487,40 +4618,40 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GO:0006936</t>
+          <t>GO:0046928</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>muscle contraction</t>
+          <t>regulation of neurotransmitter secretion</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-3.0626179646</v>
+        <v>-2.798341248</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>4/92</t>
+          <t>3/39</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596,13011</t>
+          <t>18750,68404,78771</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1,Cst7</t>
+          <t>Prkca,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3530,40 +4661,40 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GO:0006936</t>
+          <t>GO:0050804</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>muscle contraction</t>
+          <t>modulation of chemical synaptic transmission</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>-3.0626179646</v>
+        <v>-2.329226112</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>4/92</t>
+          <t>5/184</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>18750,20496,68404,78771,225872</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Nrn1,Mctp1,Npas4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3573,40 +4704,40 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GO:0090257</t>
+          <t>GO:0099177</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>regulation of muscle system process</t>
+          <t>regulation of trans-synaptic signaling</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>-2.8793781124</v>
+        <v>-2.3192671017</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>4/103</t>
+          <t>5/185</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>18750,20496,68404,78771,225872</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Nrn1,Mctp1,Npas4</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3616,76 +4747,76 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GO:0006937</t>
+          <t>GO:0060627</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>regulation of muscle contraction</t>
+          <t>regulation of vesicle-mediated transport</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-2.717951336</v>
+        <v>-2.0575374034</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3/53</t>
+          <t>6/301</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>18750,52076,60596</t>
+          <t>11981,18750,23969,68404,78771,210789</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Prkca,Tmem38b,Gucy1a1</t>
+          <t>Atp9a,Prkca,Pacsin1,Nrn1,Mctp1,Tbc1d4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>3_Summary</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>KEGG Pathway</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GO:0044057</t>
+          <t>mmu04970</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>regulation of system process</t>
+          <t>Salivary secretion</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-2.5664519338</v>
+        <v>-3.0509708137</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>5/208</t>
+          <t>3/32</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>13011,18750,22138,52076,60596</t>
+          <t>18750,20496,60596,11468,13011,13654,22138</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Cst7,Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Gucy1a1,Actg2,Cst7,Egr2,Ttn</t>
         </is>
       </c>
     </row>
@@ -3697,38 +4828,38 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>KEGG Pathway</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>GO:0003012</t>
+          <t>mmu04970</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>muscle system process</t>
+          <t>Salivary secretion</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>-2.2867765819</v>
+        <v>-3.0509708137</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>4/150</t>
+          <t>3/32</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>18750,20496,60596</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Gucy1a1</t>
         </is>
       </c>
     </row>
@@ -3740,38 +4871,38 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>KEGG Pathway</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>GO:0060047</t>
+          <t>mmu04270</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>heart contraction</t>
+          <t>Vascular smooth muscle contraction</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>-2.2729758637</v>
+        <v>-2.3257646851</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3/76</t>
+          <t>3/57</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>18750,22138,52076</t>
+          <t>11468,18750,60596</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b</t>
+          <t>Actg2,Prkca,Gucy1a1</t>
         </is>
       </c>
     </row>
@@ -3788,40 +4919,40 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>GO:0003015</t>
+          <t>GO:0044057</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>heart process</t>
+          <t>regulation of system process</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>-2.1958847155</v>
+        <v>-2.1067658563</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>3/81</t>
+          <t>5/208</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>18750,22138,52076</t>
+          <t>13011,13654,18750,22138,60596</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b</t>
+          <t>Cst7,Egr2,Prkca,Ttn,Gucy1a1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>4_Summary</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3831,40 +4962,40 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>GO:0008015</t>
+          <t>GO:0060326</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>blood circulation</t>
+          <t>cell chemotaxis</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>-2.1692324347</v>
+        <v>-2.9299506954</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>4/162</t>
+          <t>4/78</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>12145,13655,18750,20496,13654,19734</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Cxcr5,Egr3,Prkca,Slc12a2,Egr2,Rgs16</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>4_Member</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3874,40 +5005,40 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>GO:0003013</t>
+          <t>GO:0060326</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>circulatory system process</t>
+          <t>cell chemotaxis</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>-2.0358196644</v>
+        <v>-2.9299506954</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>4/177</t>
+          <t>4/78</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>12145,13655,18750,20496</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Cxcr5,Egr3,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4_Summary</t>
+          <t>4_Member</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3917,33 +5048,33 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>GO:0051588</t>
+          <t>GO:0006935</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>regulation of neurotransmitter transport</t>
+          <t>chemotaxis</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>-2.9244154751</v>
+        <v>-2.7640024542</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3/45</t>
+          <t>5/146</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>14758,18750,68404,11981,23969,210789</t>
+          <t>12145,13654,13655,18750,20496</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1,Atp9a,Pacsin1,Tbc1d4</t>
+          <t>Cxcr5,Egr2,Egr3,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
@@ -3960,33 +5091,33 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>GO:0051588</t>
+          <t>GO:0042330</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>regulation of neurotransmitter transport</t>
+          <t>taxis</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>-2.9244154751</v>
+        <v>-2.725056263</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>3/45</t>
+          <t>5/149</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>14758,18750,68404</t>
+          <t>12145,13654,13655,18750,20496</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1</t>
+          <t>Cxcr5,Egr2,Egr3,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
@@ -4003,33 +5134,33 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>GO:0006836</t>
+          <t>GO:0030595</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>neurotransmitter transport</t>
+          <t>leukocyte chemotaxis</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>-2.3558677494</v>
+        <v>-2.4150626418</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>3/71</t>
+          <t>3/53</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>14758,18750,68404</t>
+          <t>12145,18750,20496</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1</t>
+          <t>Cxcr5,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
@@ -4041,45 +5172,45 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>Reactome Gene Sets</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GO:0051051</t>
+          <t>R-MMU-418594</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>negative regulation of transport</t>
+          <t>G alpha (i) signalling events</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>-2.3389916614</v>
+        <v>-2.043740344</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>5/235</t>
+          <t>3/72</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>11981,14758,18750,23969,210789</t>
+          <t>12145,18750,19734</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Atp9a,Gpm6b,Prkca,Pacsin1,Tbc1d4</t>
+          <t>Cxcr5,Prkca,Rgs16</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4_Member</t>
+          <t>5_Summary</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4089,40 +5220,40 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>GO:0001505</t>
+          <t>GO:0072593</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>regulation of neurotransmitter levels</t>
+          <t>reactive oxygen species metabolic process</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>-2.3387865705</v>
+        <v>-2.5907376671</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>3/72</t>
+          <t>3/46</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>14758,18750,68404</t>
+          <t>13058,27209,27210</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1</t>
+          <t>Cybb,Snord32a,Snord34</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4_Member</t>
+          <t>5_Member</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4132,40 +5263,40 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GO:0099504</t>
+          <t>GO:0072593</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>synaptic vesicle cycle</t>
+          <t>reactive oxygen species metabolic process</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>-2.0695671625</v>
+        <v>-2.5907376671</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>3/90</t>
+          <t>3/46</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>18750,23969,68404</t>
+          <t>13058,27209,27210</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Prkca,Pacsin1,Nrn1</t>
+          <t>Cybb,Snord32a,Snord34</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5_Summary</t>
+          <t>6_Summary</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4175,40 +5306,40 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GO:1903530</t>
+          <t>GO:0031175</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>regulation of secretion by cell</t>
+          <t>neuron projection development</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>-2.1408720497</v>
+        <v>-2.1990268168</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>5/262</t>
+          <t>6/281</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>11981,18750,20496,22138,68404</t>
+          <t>13654,14758,18750,23969,68404,233552</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Atp9a,Prkca,Slc12a2,Ttn,Nrn1</t>
+          <t>Egr2,Gpm6b,Prkca,Pacsin1,Nrn1,Gdpd5</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5_Member</t>
+          <t>6_Member</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4218,86 +5349,43 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>GO:1903530</t>
+          <t>GO:0031175</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>regulation of secretion by cell</t>
+          <t>neuron projection development</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>-2.1408720497</v>
+        <v>-2.1990268168</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>5/262</t>
+          <t>6/281</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>11981,18750,20496,22138,68404</t>
+          <t>13654,14758,18750,23969,68404,233552</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Atp9a,Prkca,Slc12a2,Ttn,Nrn1</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>5_Member</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>GO Biological Processes</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>GO:0051046</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>regulation of secretion</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>-2.0284943437</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>5/279</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>11981,18750,20496,22138,68404</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Atp9a,Prkca,Slc12a2,Ttn,Nrn1</t>
+          <t>Egr2,Gpm6b,Prkca,Pacsin1,Nrn1,Gdpd5</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C30">
+  <conditionalFormatting sqref="C2:C29">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A29">
+  <conditionalFormatting sqref="A2:A28">
     <cfRule type="expression" priority="2" dxfId="3" stopIfTrue="0">
       <formula>RIGHT(A2,1)="y"</formula>
     </cfRule>
@@ -4305,7 +5393,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E29">
+  <conditionalFormatting sqref="E2:E28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="-6"/>
@@ -4317,7 +5405,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F29">
+  <conditionalFormatting sqref="F2:F28">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="-6"/>

</xml_diff>

<commit_message>
Adjusted DGE models and Updated figures
</commit_message>
<xml_diff>
--- a/bulkRNAseq_analyses/METASCAPE/SupplementaryFigure3g_cluster3.spleen.up_metascape_result.xlsx
+++ b/bulkRNAseq_analyses/METASCAPE/SupplementaryFigure3g_cluster3.spleen.up_metascape_result.xlsx
@@ -534,7 +534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,7 +545,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>GeneSymbol</t>
+          <t>MyList</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -580,34 +580,39 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>ko04970 Salivary secretion</t>
+          <t>GO:0051588 regulation of neurotransmitter</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>GO:0006936 muscle contraction</t>
+          <t>mmu04970 Salivary secretion</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>GO:0051588 regulation of neurotransmitter</t>
+          <t>GO:0060326 cell chemotaxis</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>GO:1903530 regulation of secretion by cel</t>
+          <t>GO:0072593 reactive oxygen species metabo</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>GO:0031175 neuron projection development</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dlg3</t>
+          <t>Cd200</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>53310</t>
+          <t>17470</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -622,7 +627,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>53310</t>
+          <t>17470</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -637,7 +642,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -651,6 +656,11 @@
         </is>
       </c>
       <c r="K2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -659,12 +669,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rec8</t>
+          <t>Egr2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>56739</t>
+          <t>13654</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -679,7 +689,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>56739</t>
+          <t>13654</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -699,29 +709,34 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>0.0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tmem38b</t>
+          <t>Npas4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>52076</t>
+          <t>225872</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -736,7 +751,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>52076</t>
+          <t>225872</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -756,7 +771,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -765,6 +780,11 @@
         </is>
       </c>
       <c r="K4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -773,12 +793,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Slc12a2</t>
+          <t>Actg2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>20496</t>
+          <t>11468</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -793,7 +813,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20496</t>
+          <t>11468</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -803,19 +823,19 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>0.0</t>
@@ -823,19 +843,24 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Slc7a10</t>
+          <t>Egr3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>53896</t>
+          <t>13655</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -850,7 +875,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>53896</t>
+          <t>13655</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -875,10 +900,15 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -887,12 +917,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tiam1</t>
+          <t>Ighd</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21844</t>
+          <t>380797</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -907,7 +937,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>21844</t>
+          <t>380797</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -936,6 +966,11 @@
         </is>
       </c>
       <c r="K7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -944,12 +979,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Rragd</t>
+          <t>Scarna13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>52187</t>
+          <t>100306943</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -964,7 +999,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>52187</t>
+          <t>100306943</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -993,6 +1028,11 @@
         </is>
       </c>
       <c r="K8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1001,12 +1041,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Atp9a</t>
+          <t>Gm22442</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11981</t>
+          <t>115487906</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1021,7 +1061,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>11981</t>
+          <t>115487906</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1046,24 +1086,29 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Prag1</t>
+          <t>Gpm6b</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>244418</t>
+          <t>14758</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1078,7 +1123,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>244418</t>
+          <t>14758</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1093,7 +1138,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1109,23 +1154,28 @@
       <c r="K10" t="inlineStr">
         <is>
           <t>0.0</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Fam160a1</t>
+          <t>Ddx43</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>229488</t>
+          <t>100048658</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>gene_synonym</t>
+          <t>symbol</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1135,7 +1185,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>229488</t>
+          <t>100048658</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1164,6 +1214,11 @@
         </is>
       </c>
       <c r="K11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1172,12 +1227,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ttn</t>
+          <t>Dlg3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>22138</t>
+          <t>53310</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1192,7 +1247,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>22138</t>
+          <t>53310</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1202,7 +1257,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1212,7 +1267,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1222,19 +1277,24 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Usp11</t>
+          <t>Rec8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>236733</t>
+          <t>56739</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1249,7 +1309,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>236733</t>
+          <t>56739</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1278,6 +1338,11 @@
         </is>
       </c>
       <c r="K13" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1286,12 +1351,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Arhgap39</t>
+          <t>Prkca</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>223666</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1306,7 +1371,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>223666</t>
+          <t>18750</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1321,34 +1386,39 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>0.0</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>1.0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tbc1d4</t>
+          <t>Zfp827</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>210789</t>
+          <t>622675</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1363,7 +1433,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>210789</t>
+          <t>622675</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1388,10 +1458,15 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1400,12 +1475,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nrn1</t>
+          <t>Pacsin1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>68404</t>
+          <t>23969</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1420,7 +1495,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>68404</t>
+          <t>23969</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1435,7 +1510,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1445,10 +1520,15 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
@@ -1457,12 +1537,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hivep3</t>
+          <t>Cybb</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16656</t>
+          <t>13058</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1477,7 +1557,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>16656</t>
+          <t>13058</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1506,6 +1586,11 @@
         </is>
       </c>
       <c r="K17" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1514,12 +1599,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cst7</t>
+          <t>Nrn1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>13011</t>
+          <t>68404</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1534,7 +1619,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13011</t>
+          <t>68404</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1544,39 +1629,44 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="I18" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>1.0</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Gdpd5</t>
+          <t>Tspan3</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>233552</t>
+          <t>56434</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1591,7 +1681,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>233552</t>
+          <t>56434</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1620,6 +1710,11 @@
         </is>
       </c>
       <c r="K19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1628,12 +1723,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Naip6</t>
+          <t>Bmyc</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17952</t>
+          <t>107771</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1648,7 +1743,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>17952</t>
+          <t>107771</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1658,7 +1753,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1677,6 +1772,11 @@
         </is>
       </c>
       <c r="K20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1685,12 +1785,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Naip5</t>
+          <t>Ephx1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17951</t>
+          <t>13849</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1705,7 +1805,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>17951</t>
+          <t>13849</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1715,7 +1815,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1734,6 +1834,11 @@
         </is>
       </c>
       <c r="K21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1742,12 +1847,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gm3739</t>
+          <t>Ppat</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>100042235</t>
+          <t>231327</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1762,7 +1867,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>100042235</t>
+          <t>231327</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1791,6 +1896,11 @@
         </is>
       </c>
       <c r="K22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1799,12 +1909,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Clip2</t>
+          <t>Cbx6</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>269713</t>
+          <t>494448</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1819,7 +1929,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>269713</t>
+          <t>494448</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1848,6 +1958,11 @@
         </is>
       </c>
       <c r="K23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1856,12 +1971,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Tnfrsf8</t>
+          <t>Izumo1r</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21941</t>
+          <t>64931</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1876,7 +1991,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>21941</t>
+          <t>64931</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1905,6 +2020,11 @@
         </is>
       </c>
       <c r="K24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1913,12 +2033,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Npas4</t>
+          <t>Cul7</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>225872</t>
+          <t>66515</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1933,7 +2053,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>225872</t>
+          <t>66515</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1962,6 +2082,11 @@
         </is>
       </c>
       <c r="K25" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -1970,17 +2095,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Gucy1a3</t>
+          <t>Cxcr5</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>60596</t>
+          <t>12145</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>gene_synonym</t>
+          <t>symbol</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1990,7 +2115,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>60596</t>
+          <t>12145</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2005,20 +2130,25 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
       <c r="K26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2027,12 +2157,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ighd</t>
+          <t>Usp11</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>380797</t>
+          <t>236733</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2047,7 +2177,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>380797</t>
+          <t>236733</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2076,6 +2206,11 @@
         </is>
       </c>
       <c r="K27" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2084,12 +2219,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Gpm6b</t>
+          <t>Arhgap39</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>14758</t>
+          <t>223666</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2104,7 +2239,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>14758</t>
+          <t>223666</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2119,7 +2254,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2129,10 +2264,15 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2141,12 +2281,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Ddx43</t>
+          <t>Gm26202</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>100048658</t>
+          <t>115488998</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2161,7 +2301,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>100048658</t>
+          <t>115488998</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2190,6 +2330,11 @@
         </is>
       </c>
       <c r="K29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2198,49 +2343,74 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Gm17173</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
+          <t>Snord82</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>80828</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>80828</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>H2-Oa</t>
+          <t>Snord87</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>15001</t>
+          <t>266793</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2255,7 +2425,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>15001</t>
+          <t>266793</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2284,6 +2454,11 @@
         </is>
       </c>
       <c r="K31" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2292,12 +2467,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tspan3</t>
+          <t>Snord32a</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>56434</t>
+          <t>27209</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2312,7 +2487,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>56434</t>
+          <t>27209</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2341,6 +2516,11 @@
         </is>
       </c>
       <c r="K32" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2349,12 +2529,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bmyc</t>
+          <t>Snord34</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>107771</t>
+          <t>27210</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2369,7 +2549,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>107771</t>
+          <t>27210</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2398,6 +2578,11 @@
         </is>
       </c>
       <c r="K33" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2406,12 +2591,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Ephx1</t>
+          <t>Tbc1d4</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13849</t>
+          <t>210789</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2426,7 +2611,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>13849</t>
+          <t>210789</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2441,7 +2626,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2455,6 +2640,11 @@
         </is>
       </c>
       <c r="K34" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2463,12 +2653,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Ppat</t>
+          <t>Gm3739</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>231327</t>
+          <t>100042235</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2483,7 +2673,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>231327</t>
+          <t>100042235</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2512,6 +2702,11 @@
         </is>
       </c>
       <c r="K35" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2520,12 +2715,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Cbx6</t>
+          <t>Hivep3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>494448</t>
+          <t>16656</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2540,7 +2735,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>494448</t>
+          <t>16656</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2569,6 +2764,11 @@
         </is>
       </c>
       <c r="K36" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2577,12 +2777,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Izumo1r</t>
+          <t>Cst7</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>64931</t>
+          <t>13011</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2597,7 +2797,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>64931</t>
+          <t>13011</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2607,7 +2807,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2617,7 +2817,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2626,6 +2826,11 @@
         </is>
       </c>
       <c r="K37" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2634,12 +2839,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Cybb</t>
+          <t>Chn2</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>13058</t>
+          <t>69993</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2654,7 +2859,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>13058</t>
+          <t>69993</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2669,7 +2874,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2683,6 +2888,11 @@
         </is>
       </c>
       <c r="K38" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2691,12 +2901,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Cxcr5</t>
+          <t>Slc12a2</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>12145</t>
+          <t>20496</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2711,7 +2921,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>12145</t>
+          <t>20496</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2721,7 +2931,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2731,15 +2941,20 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2748,12 +2963,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Prkca</t>
+          <t>Slc7a10</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>18750</t>
+          <t>53896</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2768,7 +2983,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>18750</t>
+          <t>53896</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2783,34 +2998,39 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Zfp827</t>
+          <t>Naip6</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>622675</t>
+          <t>17952</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2825,7 +3045,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>622675</t>
+          <t>17952</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2835,7 +3055,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2854,6 +3074,11 @@
         </is>
       </c>
       <c r="K41" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
@@ -2862,12 +3087,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Pacsin1</t>
+          <t>Naip5</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>23969</t>
+          <t>17951</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2882,7 +3107,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>23969</t>
+          <t>17951</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2892,7 +3117,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2907,22 +3132,917 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Gdpd5</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>233552</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>233552</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Atp9a</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>11981</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>11981</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Rgs16</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>19734</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>19734</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Mctp1</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>78771</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>78771</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Myo1h</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>231646</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>231646</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Chst15</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>77590</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>77590</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Gucy1a3</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>60596</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>gene_synonym</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>60596</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Prag1</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>244418</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>244418</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Rragd</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>52187</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>52187</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Gm37347</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>AC154627.3</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Tnfrsf8</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>21941</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>21941</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Susd2</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>71733</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>71733</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Fam160a1</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>229488</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>gene_synonym</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>229488</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ttn</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>22138</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>22138</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>M. musculus</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E42">
+  <conditionalFormatting sqref="E2:E57">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G57">
     <cfRule type="cellIs" priority="2" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2933,7 +4053,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H42">
+  <conditionalFormatting sqref="H2:H57">
     <cfRule type="cellIs" priority="5" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2944,7 +4064,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I42">
+  <conditionalFormatting sqref="I2:I57">
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2955,7 +4075,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J42">
+  <conditionalFormatting sqref="J2:J57">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2966,7 +4086,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K42">
+  <conditionalFormatting sqref="K2:K57">
     <cfRule type="cellIs" priority="14" operator="equal" dxfId="1" stopIfTrue="0">
       <formula>1</formula>
     </cfRule>
@@ -2974,6 +4094,17 @@
       <formula>"1"</formula>
     </cfRule>
     <cfRule type="expression" priority="16" dxfId="2" stopIfTrue="1">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L57">
+    <cfRule type="cellIs" priority="17" operator="equal" dxfId="1" stopIfTrue="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="18" operator="equal" dxfId="1" stopIfTrue="0">
+      <formula>"1"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="19" dxfId="2" stopIfTrue="1">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2989,7 +4120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3066,14 +4197,14 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>-4.1199323855</v>
+        <v>-3.8865642647</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4/49</t>
+          <t>4/44</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -3109,14 +4240,14 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-4.1199323855</v>
+        <v>-3.8865642647</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4/49</t>
+          <t>4/44</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -3152,7 +4283,7 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-2.542707383</v>
+        <v>-2.2431293242</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
@@ -3195,7 +4326,7 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>-2.3219637852</v>
+        <v>-2.0273283633</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -3219,7 +4350,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1_Member</t>
+          <t>2_Summary</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3229,76 +4360,76 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>GO:0010466</t>
+          <t>GO:0051588</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>negative regulation of peptidase activity</t>
+          <t>regulation of neurotransmitter transport</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>-2.1521158653</v>
+        <v>-3.8480472385</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3/84</t>
+          <t>4/45</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>13011,17951,17952</t>
+          <t>14758,18750,68404,78771,11981,17470,23969,210789,20496,22138,225872</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Cst7,Naip5,Naip6</t>
+          <t>Gpm6b,Prkca,Nrn1,Mctp1,Atp9a,Cd200,Pacsin1,Tbc1d4,Slc12a2,Ttn,Npas4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2_Summary</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>KEGG Pathway</t>
+          <t>GO Biological Processes</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ko04970</t>
+          <t>GO:0051588</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Salivary secretion</t>
+          <t>regulation of neurotransmitter transport</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>-3.3626075359</v>
+        <v>-3.8480472385</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3/32</t>
+          <t>4/45</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>18750,20496,60596,13058,14758,52076,12145</t>
+          <t>14758,18750,68404,78771</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Prkca,Slc12a2,Gucy1a1,Cybb,Gpm6b,Tmem38b,Cxcr5</t>
+          <t>Gpm6b,Prkca,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
@@ -3310,38 +4441,38 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KEGG Pathway</t>
+          <t>GO Biological Processes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ko04970</t>
+          <t>GO:0051051</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Salivary secretion</t>
+          <t>negative regulation of transport</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-3.3626075359</v>
+        <v>-3.3411377526</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3/32</t>
+          <t>7/235</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>18750,20496,60596</t>
+          <t>11981,14758,17470,18750,23969,78771,210789</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Prkca,Slc12a2,Gucy1a1</t>
+          <t>Atp9a,Gpm6b,Cd200,Prkca,Pacsin1,Mctp1,Tbc1d4</t>
         </is>
       </c>
     </row>
@@ -3353,38 +4484,38 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>KEGG Pathway</t>
+          <t>GO Biological Processes</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mmu04970</t>
+          <t>GO:0001505</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Salivary secretion</t>
+          <t>regulation of neurotransmitter levels</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>-3.322624285</v>
+        <v>-3.0833540895</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3/33</t>
+          <t>4/71</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>18750,20496,60596</t>
+          <t>14758,18750,68404,78771</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Prkca,Slc12a2,Gucy1a1</t>
+          <t>Gpm6b,Prkca,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
@@ -3401,33 +4532,33 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GO:0043269</t>
+          <t>GO:1903530</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>regulation of ion transport</t>
+          <t>regulation of secretion by cell</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>-2.270018949</v>
+        <v>-3.0596733891</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>5/244</t>
+          <t>7/262</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>13058,14758,18750,20496,52076</t>
+          <t>11981,17470,18750,20496,22138,68404,78771</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Cybb,Gpm6b,Prkca,Slc12a2,Tmem38b</t>
+          <t>Atp9a,Cd200,Prkca,Slc12a2,Ttn,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
@@ -3444,40 +4575,40 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GO:0030595</t>
+          <t>GO:0051046</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>leukocyte chemotaxis</t>
+          <t>regulation of secretion</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>-2.0178765907</v>
+        <v>-2.8999295696</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3/94</t>
+          <t>7/279</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>12145,18750,20496</t>
+          <t>11981,17470,18750,20496,22138,68404,78771</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Cxcr5,Prkca,Slc12a2</t>
+          <t>Atp9a,Cd200,Prkca,Slc12a2,Ttn,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3_Summary</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3487,40 +4618,40 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GO:0006936</t>
+          <t>GO:0046928</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>muscle contraction</t>
+          <t>regulation of neurotransmitter secretion</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-3.0626179646</v>
+        <v>-2.798341248</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>4/92</t>
+          <t>3/39</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596,13011</t>
+          <t>18750,68404,78771</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1,Cst7</t>
+          <t>Prkca,Nrn1,Mctp1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3530,40 +4661,40 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GO:0006936</t>
+          <t>GO:0050804</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>muscle contraction</t>
+          <t>modulation of chemical synaptic transmission</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>-3.0626179646</v>
+        <v>-2.329226112</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>4/92</t>
+          <t>5/184</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>18750,20496,68404,78771,225872</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Nrn1,Mctp1,Npas4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3573,40 +4704,40 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GO:0090257</t>
+          <t>GO:0099177</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>regulation of muscle system process</t>
+          <t>regulation of trans-synaptic signaling</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>-2.8793781124</v>
+        <v>-2.3192671017</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>4/103</t>
+          <t>5/185</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>18750,20496,68404,78771,225872</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Nrn1,Mctp1,Npas4</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>2_Member</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3616,76 +4747,76 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GO:0006937</t>
+          <t>GO:0060627</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>regulation of muscle contraction</t>
+          <t>regulation of vesicle-mediated transport</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-2.717951336</v>
+        <v>-2.0575374034</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3/53</t>
+          <t>6/301</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>18750,52076,60596</t>
+          <t>11981,18750,23969,68404,78771,210789</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Prkca,Tmem38b,Gucy1a1</t>
+          <t>Atp9a,Prkca,Pacsin1,Nrn1,Mctp1,Tbc1d4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>3_Summary</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>KEGG Pathway</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GO:0044057</t>
+          <t>mmu04970</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>regulation of system process</t>
+          <t>Salivary secretion</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-2.5664519338</v>
+        <v>-3.0509708137</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>5/208</t>
+          <t>3/32</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>13011,18750,22138,52076,60596</t>
+          <t>18750,20496,60596,11468,13011,13654,22138</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Cst7,Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Gucy1a1,Actg2,Cst7,Egr2,Ttn</t>
         </is>
       </c>
     </row>
@@ -3697,38 +4828,38 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>KEGG Pathway</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>GO:0003012</t>
+          <t>mmu04970</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>muscle system process</t>
+          <t>Salivary secretion</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>-2.2867765819</v>
+        <v>-3.0509708137</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>4/150</t>
+          <t>3/32</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>18750,20496,60596</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Prkca,Slc12a2,Gucy1a1</t>
         </is>
       </c>
     </row>
@@ -3740,38 +4871,38 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>KEGG Pathway</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>GO:0060047</t>
+          <t>mmu04270</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>heart contraction</t>
+          <t>Vascular smooth muscle contraction</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>-2.2729758637</v>
+        <v>-2.3257646851</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3/76</t>
+          <t>3/57</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>18750,22138,52076</t>
+          <t>11468,18750,60596</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b</t>
+          <t>Actg2,Prkca,Gucy1a1</t>
         </is>
       </c>
     </row>
@@ -3788,40 +4919,40 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>GO:0003015</t>
+          <t>GO:0044057</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>heart process</t>
+          <t>regulation of system process</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>-2.1958847155</v>
+        <v>-2.1067658563</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>3/81</t>
+          <t>5/208</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>18750,22138,52076</t>
+          <t>13011,13654,18750,22138,60596</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b</t>
+          <t>Cst7,Egr2,Prkca,Ttn,Gucy1a1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>4_Summary</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3831,40 +4962,40 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>GO:0008015</t>
+          <t>GO:0060326</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>blood circulation</t>
+          <t>cell chemotaxis</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>-2.1692324347</v>
+        <v>-2.9299506954</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>4/162</t>
+          <t>4/78</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>12145,13655,18750,20496,13654,19734</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Cxcr5,Egr3,Prkca,Slc12a2,Egr2,Rgs16</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3_Member</t>
+          <t>4_Member</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3874,40 +5005,40 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>GO:0003013</t>
+          <t>GO:0060326</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>circulatory system process</t>
+          <t>cell chemotaxis</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>-2.0358196644</v>
+        <v>-2.9299506954</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>4/177</t>
+          <t>4/78</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>18750,22138,52076,60596</t>
+          <t>12145,13655,18750,20496</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Prkca,Ttn,Tmem38b,Gucy1a1</t>
+          <t>Cxcr5,Egr3,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4_Summary</t>
+          <t>4_Member</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3917,33 +5048,33 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>GO:0051588</t>
+          <t>GO:0006935</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>regulation of neurotransmitter transport</t>
+          <t>chemotaxis</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>-2.9244154751</v>
+        <v>-2.7640024542</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3/45</t>
+          <t>5/146</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>14758,18750,68404,11981,23969,210789</t>
+          <t>12145,13654,13655,18750,20496</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1,Atp9a,Pacsin1,Tbc1d4</t>
+          <t>Cxcr5,Egr2,Egr3,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
@@ -3960,33 +5091,33 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>GO:0051588</t>
+          <t>GO:0042330</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>regulation of neurotransmitter transport</t>
+          <t>taxis</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>-2.9244154751</v>
+        <v>-2.725056263</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>3/45</t>
+          <t>5/149</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>14758,18750,68404</t>
+          <t>12145,13654,13655,18750,20496</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1</t>
+          <t>Cxcr5,Egr2,Egr3,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
@@ -4003,33 +5134,33 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>GO:0006836</t>
+          <t>GO:0030595</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>neurotransmitter transport</t>
+          <t>leukocyte chemotaxis</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>-2.3558677494</v>
+        <v>-2.4150626418</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>3/71</t>
+          <t>3/53</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>14758,18750,68404</t>
+          <t>12145,18750,20496</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1</t>
+          <t>Cxcr5,Prkca,Slc12a2</t>
         </is>
       </c>
     </row>
@@ -4041,45 +5172,45 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>GO Biological Processes</t>
+          <t>Reactome Gene Sets</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GO:0051051</t>
+          <t>R-MMU-418594</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>negative regulation of transport</t>
+          <t>G alpha (i) signalling events</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>-2.3389916614</v>
+        <v>-2.043740344</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>5/235</t>
+          <t>3/72</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>11981,14758,18750,23969,210789</t>
+          <t>12145,18750,19734</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Atp9a,Gpm6b,Prkca,Pacsin1,Tbc1d4</t>
+          <t>Cxcr5,Prkca,Rgs16</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4_Member</t>
+          <t>5_Summary</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4089,40 +5220,40 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>GO:0001505</t>
+          <t>GO:0072593</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>regulation of neurotransmitter levels</t>
+          <t>reactive oxygen species metabolic process</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>-2.3387865705</v>
+        <v>-2.5907376671</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>3/72</t>
+          <t>3/46</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>14758,18750,68404</t>
+          <t>13058,27209,27210</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Gpm6b,Prkca,Nrn1</t>
+          <t>Cybb,Snord32a,Snord34</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4_Member</t>
+          <t>5_Member</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4132,40 +5263,40 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GO:0099504</t>
+          <t>GO:0072593</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>synaptic vesicle cycle</t>
+          <t>reactive oxygen species metabolic process</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>-2.0695671625</v>
+        <v>-2.5907376671</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>3/90</t>
+          <t>3/46</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>18750,23969,68404</t>
+          <t>13058,27209,27210</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Prkca,Pacsin1,Nrn1</t>
+          <t>Cybb,Snord32a,Snord34</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5_Summary</t>
+          <t>6_Summary</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4175,40 +5306,40 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GO:1903530</t>
+          <t>GO:0031175</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>regulation of secretion by cell</t>
+          <t>neuron projection development</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>-2.1408720497</v>
+        <v>-2.1990268168</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>5/262</t>
+          <t>6/281</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>11981,18750,20496,22138,68404</t>
+          <t>13654,14758,18750,23969,68404,233552</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Atp9a,Prkca,Slc12a2,Ttn,Nrn1</t>
+          <t>Egr2,Gpm6b,Prkca,Pacsin1,Nrn1,Gdpd5</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5_Member</t>
+          <t>6_Member</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4218,86 +5349,43 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>GO:1903530</t>
+          <t>GO:0031175</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>regulation of secretion by cell</t>
+          <t>neuron projection development</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>-2.1408720497</v>
+        <v>-2.1990268168</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>5/262</t>
+          <t>6/281</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>11981,18750,20496,22138,68404</t>
+          <t>13654,14758,18750,23969,68404,233552</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Atp9a,Prkca,Slc12a2,Ttn,Nrn1</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>5_Member</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>GO Biological Processes</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>GO:0051046</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>regulation of secretion</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>-2.0284943437</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>5/279</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>11981,18750,20496,22138,68404</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Atp9a,Prkca,Slc12a2,Ttn,Nrn1</t>
+          <t>Egr2,Gpm6b,Prkca,Pacsin1,Nrn1,Gdpd5</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C30">
+  <conditionalFormatting sqref="C2:C29">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A29">
+  <conditionalFormatting sqref="A2:A28">
     <cfRule type="expression" priority="2" dxfId="3" stopIfTrue="0">
       <formula>RIGHT(A2,1)="y"</formula>
     </cfRule>
@@ -4305,7 +5393,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E29">
+  <conditionalFormatting sqref="E2:E28">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="-6"/>
@@ -4317,7 +5405,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F29">
+  <conditionalFormatting sqref="F2:F28">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="-6"/>

</xml_diff>